<commit_message>
Update: docs covering early good end to the quest
</commit_message>
<xml_diff>
--- a/Docs/Project Managerhuh.xlsx
+++ b/Docs/Project Managerhuh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etste\Documents\Projects\Mods\Morrowind\othral-ancestral-tomb\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CAF177E1-F6A3-4339-81C0-2588833FED36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F06FAB01-DF30-46FE-B5EA-14EDC680A425}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="765" activeTab="4" xr2:uid="{4904B981-F0B7-4F9A-A77B-E04B97902615}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="408">
   <si>
     <t>Name</t>
   </si>
@@ -657,9 +657,6 @@
     <t>Journal "tlvoat_Estranged_Spirits", 31, ModDisposition 5, StartScript tlvoat_othral_quest_glb_script, Goodbye</t>
   </si>
   <si>
-    <t>tlvoat_estranged_spirits.Journal == 70</t>
-  </si>
-  <si>
     <t>I should speak with Aryasi now that she's had time to speak to her grandmother's spirit.</t>
   </si>
   <si>
@@ -945,9 +942,6 @@
     <t>Thank you %PCName. Coming here has brought up so many old feelings that I've kept so very deeply buried. It hurts all the more that I don't even hear my grandmother's spirit, as she was the only one I ever had a good relationship with. I used to suspect that there is a hidden section of the tomb, and I am once again hoping there is one and that she was laid to rest there. Though I might just be letting myself be fooled by hope once again.</t>
   </si>
   <si>
-    <t>I… Thank you %PCName… That means a lot to me. [She is silent for a minute.] I've always felt like a coward or that I was weak for running away, rather than sticking with it. Everything that I've done has been to get as far away from my family. I think I've been hurting myself. I had hoped to speak to my grandmother, but she too is silent. I once suspected that there is a hidden section in this tomb, and she's in there and that's why I can't hear her.</t>
-  </si>
-  <si>
     <t>Aryasi wants further help with speaking with her family's spirits. I have turned her down for now.</t>
   </si>
   <si>
@@ -1179,9 +1173,6 @@
     <t>They are here, as I can... sense their presence. No, they are choosing to keep me out. I am not family to them, and I haven't been for a long time.</t>
   </si>
   <si>
-    <t>IF tlvoat_hasPCReceivedReward1 = 0: Choice "You've been disowned?", 1, "I'm sorry to hear that, but I would like my gold before we continue.", 2 ELSE Choice "You've been disowned?", 1, "Before I go, is there anything else I could help with?", 3, "[Leave] Good luck with your family.", 4; set tlvoat_hasAskedAboutSpirits to 1</t>
-  </si>
-  <si>
     <t>Choice "[Let her continue.]", 10, "I wouldn't know. I didn't know my parents.", 11</t>
   </si>
   <si>
@@ -1207,9 +1198,6 @@
   </si>
   <si>
     <t>Honestly that sounds like a blessing from the Tribunal. No one to judge you, no one to control you. You're free from the burden of lingering pain of what could, should, have been.</t>
-  </si>
-  <si>
-    <t>if PC in Temple: Choice "I'm sorry to hear that your family pushed you away.", 20, "Was there anyone in your family who you had a good relationship with?", 21, "Just as Ghostfence is a monument to Dunmer pride in overcoming our enemies, so too should you in standing up for yourself against a family that should know better.", 22 ELSE Choice "I'm sorry to hear that your family pushed you away.", 20, "Was there anyone in your family who you had a good relationship with?", 21</t>
   </si>
   <si>
     <t>Choice "What happened?", 10, "No one to love you. No happy memories.", 12, "That sounds like, despite the pain, you have some happy memories?", 13</t>
@@ -1241,9 +1229,6 @@
     <t>I hadn't thought about it like that. [A look of contemplation passes over her face, before easing into a lighter expression.] Thank you sera %PCName for being patient with me and hearing me out.</t>
   </si>
   <si>
-    <t>Thank you sera %PCName, I hope that's true. There's so much more that I want to do, but never felt like I could stick with it.</t>
-  </si>
-  <si>
     <t>RemoveItem Gold_001, 70; Player-&gt;AddItem Gold_001, 70; set tlvoat_hasPCReceivedReward1; Choice "So, your family. They don't like you very much?", 1, "Before I go, is there anything else I could help with?", 3, "[Leave] Good luck with your family.", 4</t>
   </si>
   <si>
@@ -1254,6 +1239,39 @@
   </si>
   <si>
     <t>tlvoat_Estranged_Spirits.journal == 105</t>
+  </si>
+  <si>
+    <t>tlvoat_Estarnged_Spirits.Journal &gt;= 30, tlvoat_Estarnged_Spirits.Journal &lt;= 45, tlvoat_Othral_Disturb1_State == 1</t>
+  </si>
+  <si>
+    <t>What are you DOING? Just because my family has pushed me away does NOT mean that I'm fine with having their remains disturbed. I need you to leave. NOW!</t>
+  </si>
+  <si>
+    <t>ModDisposition -100, Journal "tlvoat_Estranged_Spirits", 150; StopScript "tlvoat_othral_quest_glb_script"; Goodbye</t>
+  </si>
+  <si>
+    <t>Why would you do that? What is wrong with you? You need to leave.</t>
+  </si>
+  <si>
+    <t>tlvoat_estranged_spirits.Journal == 60, tlvoat_Othral_Disturb2_State == 1</t>
+  </si>
+  <si>
+    <t>tlvoat_estranged_spirits.Journal &gt; 70</t>
+  </si>
+  <si>
+    <t>Did you lead me here just to make me watch as you disturbed my grandmother's remains? You are a sick and cruel person %PCName. Leave this place.</t>
+  </si>
+  <si>
+    <t>IF tlvoat_hasPCReceivedReward1 = 0: Choice "You've been disowned?", 1, "I'm sorry to hear that, but I would like my gold before we continue.", 2 ELSE Choice "You've been disowned?", 1, "I'm sorry to hear that. Before I go, is there anything else I could help with?", 3, "[Leave] Good luck with your family.", 4; set tlvoat_hasAskedAboutSpirits to 1</t>
+  </si>
+  <si>
+    <t>if PC in Temple: Choice "I'm sorry to hear that your family pushed you away.", 20, "Was there anyone in your family who you had a good relationship with?", 21, "Just as Ghostfence is a monument to Dunmer pride in overcoming our enemies, so too should you in staying true to yourself and doing what you must.", 22 ELSE Choice "I'm sorry to hear that your family pushed you away.", 20, "Was there anyone in your family who you had a good relationship with?", 21</t>
+  </si>
+  <si>
+    <t>I… Thank you %PCName… That means a lot to me. [She is silent for a minute.] I'd always felt like a coward or that I was weak for running away, rather than sticking with it. It had just become so unbearable that I thought I'd never want to see them again, and yet I've come back here. Hoping. I had hoped to speak to my grandmother, but she too is silent. I had once suspected that there is a hidden section in this tomb. That I can't hear her because she's there.</t>
+  </si>
+  <si>
+    <t>Thank you sera %PCName, I hope that's true. There's so much more that I want to do, but never felt like I could stick with it. Because right now, I'm a bit of a failure. Even if my family's spirits spoke to me they'd be disappointed that I haven't dedicated myself to anything. When the going gets tough I move to a new town, or guild, or job. Not staying long enough to even leave behind any friends or lovers. I want to speak to grandmother, but I'm scared of what she'd think of me. Of what she'd say.</t>
   </si>
 </sst>
 </file>
@@ -1869,7 +1887,7 @@
   <dimension ref="A2:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2014,7 +2032,7 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C10" t="s">
         <v>13</v>
@@ -2023,7 +2041,7 @@
         <v>60</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
   </sheetData>
@@ -2153,7 +2171,7 @@
   <dimension ref="A2:F24"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2236,7 +2254,7 @@
         <v>27</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D6">
         <v>30</v>
@@ -2256,7 +2274,7 @@
         <v>27</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D7">
         <v>31</v>
@@ -2276,7 +2294,7 @@
         <v>27</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D8">
         <v>35</v>
@@ -2290,7 +2308,7 @@
         <v>27</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D9">
         <v>40</v>
@@ -2307,7 +2325,7 @@
         <v>27</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D10">
         <v>45</v>
@@ -2321,7 +2339,7 @@
         <v>27</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D11">
         <v>50</v>
@@ -2338,7 +2356,7 @@
         <v>27</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D12">
         <v>60</v>
@@ -2352,13 +2370,13 @@
         <v>27</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D13">
         <v>70</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -2369,7 +2387,7 @@
         <v>27</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D14">
         <v>100</v>
@@ -2403,7 +2421,7 @@
         <v>27</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="D16">
         <v>105</v>
@@ -2417,7 +2435,7 @@
         <v>27</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D17">
         <v>150</v>
@@ -2494,7 +2512,7 @@
         <v>27</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D21">
         <v>500</v>
@@ -2511,7 +2529,7 @@
         <v>27</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D22">
         <v>600</v>
@@ -2528,7 +2546,7 @@
         <v>27</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D23">
         <v>700</v>
@@ -2545,7 +2563,7 @@
         <v>27</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D24">
         <v>701</v>
@@ -2847,10 +2865,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87FFBF93-1C76-46C0-825C-97FF26B47D4C}">
-  <dimension ref="A2:F107"/>
+  <dimension ref="A2:F110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="F78" sqref="F78"/>
+    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
+      <selection activeCell="D108" sqref="D108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2930,7 +2948,7 @@
         <v>110</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F5" t="s">
         <v>140</v>
@@ -2947,7 +2965,7 @@
         <v>110</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="F6" t="s">
         <v>141</v>
@@ -2964,7 +2982,7 @@
         <v>110</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F7" t="s">
         <v>142</v>
@@ -2981,7 +2999,7 @@
         <v>110</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F8" t="s">
         <v>143</v>
@@ -2998,7 +3016,7 @@
         <v>110</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F9" t="s">
         <v>150</v>
@@ -3015,10 +3033,10 @@
         <v>110</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F10" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -3032,10 +3050,10 @@
         <v>110</v>
       </c>
       <c r="D11" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="F11" t="s">
         <v>231</v>
-      </c>
-      <c r="F11" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3083,13 +3101,13 @@
         <v>110</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>113</v>
       </c>
       <c r="F14" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -3103,13 +3121,13 @@
         <v>110</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>113</v>
       </c>
       <c r="F15" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3123,13 +3141,13 @@
         <v>110</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="F16" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -3143,13 +3161,13 @@
         <v>110</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="F17" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3163,13 +3181,16 @@
         <v>110</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>161</v>
+        <v>398</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>347</v>
       </c>
       <c r="F18" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -3180,13 +3201,13 @@
         <v>110</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>307</v>
+        <v>161</v>
       </c>
       <c r="F19" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>14</v>
       </c>
@@ -3197,10 +3218,10 @@
         <v>110</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>237</v>
+        <v>305</v>
       </c>
       <c r="F20" t="s">
-        <v>236</v>
+        <v>304</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3214,10 +3235,10 @@
         <v>110</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>173</v>
+        <v>236</v>
       </c>
       <c r="F21" t="s">
-        <v>291</v>
+        <v>235</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3231,13 +3252,13 @@
         <v>110</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>318</v>
+        <v>173</v>
       </c>
       <c r="F22" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>14</v>
       </c>
@@ -3248,13 +3269,13 @@
         <v>110</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>174</v>
+        <v>316</v>
       </c>
       <c r="F23" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>14</v>
       </c>
@@ -3265,13 +3286,13 @@
         <v>110</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>238</v>
+        <v>174</v>
       </c>
       <c r="F24" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>14</v>
       </c>
@@ -3282,16 +3303,13 @@
         <v>110</v>
       </c>
       <c r="D25" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="F25" t="s">
         <v>239</v>
       </c>
-      <c r="E25" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="F25" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>14</v>
       </c>
@@ -3302,16 +3320,16 @@
         <v>110</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>360</v>
+        <v>238</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>352</v>
+        <v>113</v>
       </c>
       <c r="F26" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>14</v>
       </c>
@@ -3322,16 +3340,16 @@
         <v>110</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>241</v>
+        <v>403</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>113</v>
+        <v>399</v>
       </c>
       <c r="F27" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>14</v>
       </c>
@@ -3342,16 +3360,16 @@
         <v>110</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>348</v>
+        <v>358</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="F28" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -3362,13 +3380,16 @@
         <v>110</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>113</v>
       </c>
       <c r="F29" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>14</v>
       </c>
@@ -3379,13 +3400,16 @@
         <v>110</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>314</v>
+        <v>346</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>347</v>
       </c>
       <c r="F30" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>14</v>
       </c>
@@ -3396,16 +3420,13 @@
         <v>110</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>346</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>113</v>
+        <v>241</v>
       </c>
       <c r="F31" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>14</v>
       </c>
@@ -3416,73 +3437,70 @@
         <v>110</v>
       </c>
       <c r="D32" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="F32" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>14</v>
+      </c>
+      <c r="B33" t="s">
+        <v>29</v>
+      </c>
+      <c r="C33" t="s">
+        <v>110</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="F33" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>14</v>
+      </c>
+      <c r="B34" t="s">
+        <v>29</v>
+      </c>
+      <c r="C34" t="s">
+        <v>110</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F34" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>14</v>
+      </c>
+      <c r="B35" t="s">
+        <v>29</v>
+      </c>
+      <c r="C35" t="s">
+        <v>110</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="F35" t="s">
         <v>243</v>
       </c>
-      <c r="F32" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>14</v>
-      </c>
-      <c r="B33" t="s">
-        <v>29</v>
-      </c>
-      <c r="C33" t="s">
-        <v>103</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>329</v>
-      </c>
-      <c r="F33" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>14</v>
-      </c>
-      <c r="B34" t="s">
-        <v>29</v>
-      </c>
-      <c r="C34" t="s">
-        <v>103</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="F34" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>14</v>
-      </c>
-      <c r="B35" t="s">
-        <v>29</v>
-      </c>
-      <c r="C35" t="s">
-        <v>103</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="F35" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>14</v>
       </c>
@@ -3493,16 +3511,16 @@
         <v>103</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>183</v>
+        <v>245</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>151</v>
+        <v>327</v>
       </c>
       <c r="F36" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>14</v>
       </c>
@@ -3513,16 +3531,16 @@
         <v>103</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>155</v>
+        <v>182</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>190</v>
+        <v>328</v>
       </c>
       <c r="F37" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>14</v>
       </c>
@@ -3533,13 +3551,16 @@
         <v>103</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>156</v>
+        <v>149</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>151</v>
       </c>
       <c r="F38" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>14</v>
       </c>
@@ -3550,16 +3571,16 @@
         <v>103</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>253</v>
+        <v>183</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>189</v>
+        <v>151</v>
       </c>
       <c r="F39" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>14</v>
       </c>
@@ -3570,13 +3591,16 @@
         <v>103</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>188</v>
+        <v>155</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>190</v>
       </c>
       <c r="F40" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>14</v>
       </c>
@@ -3587,13 +3611,10 @@
         <v>103</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>201</v>
+        <v>156</v>
       </c>
       <c r="F41" t="s">
-        <v>185</v>
+        <v>154</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3607,16 +3628,16 @@
         <v>103</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>186</v>
+        <v>252</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>202</v>
+        <v>189</v>
       </c>
       <c r="F42" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>14</v>
       </c>
@@ -3627,16 +3648,13 @@
         <v>103</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>361</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>325</v>
+        <v>188</v>
       </c>
       <c r="F43" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>14</v>
       </c>
@@ -3647,16 +3665,16 @@
         <v>103</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>324</v>
+        <v>186</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>331</v>
+        <v>201</v>
       </c>
       <c r="F44" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>14</v>
       </c>
@@ -3667,13 +3685,13 @@
         <v>103</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>362</v>
+        <v>186</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>332</v>
+        <v>202</v>
       </c>
       <c r="F45" t="s">
-        <v>320</v>
+        <v>187</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3687,16 +3705,16 @@
         <v>103</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>373</v>
+        <v>359</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>372</v>
+        <v>323</v>
       </c>
       <c r="F46" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>14</v>
       </c>
@@ -3707,16 +3725,16 @@
         <v>103</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>245</v>
+        <v>322</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>323</v>
+        <v>329</v>
       </c>
       <c r="F47" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>14</v>
       </c>
@@ -3727,16 +3745,16 @@
         <v>103</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>322</v>
+        <v>360</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>323</v>
+        <v>330</v>
       </c>
       <c r="F48" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>14</v>
       </c>
@@ -3747,16 +3765,16 @@
         <v>103</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>251</v>
+        <v>371</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="F49" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>14</v>
       </c>
@@ -3767,16 +3785,16 @@
         <v>103</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>375</v>
+        <v>321</v>
       </c>
       <c r="F50" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>14</v>
       </c>
@@ -3787,10 +3805,13 @@
         <v>103</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>247</v>
+        <v>320</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>321</v>
       </c>
       <c r="F51" t="s">
-        <v>248</v>
+        <v>150</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3804,13 +3825,13 @@
         <v>103</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="F52" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3824,16 +3845,16 @@
         <v>103</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="F53" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>14</v>
       </c>
@@ -3844,13 +3865,10 @@
         <v>103</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>333</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>327</v>
+        <v>246</v>
       </c>
       <c r="F54" t="s">
-        <v>334</v>
+        <v>247</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3864,13 +3882,13 @@
         <v>103</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>326</v>
+        <v>248</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>327</v>
+        <v>373</v>
       </c>
       <c r="F55" t="s">
-        <v>328</v>
+        <v>294</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3884,13 +3902,13 @@
         <v>103</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>336</v>
+        <v>249</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>297</v>
+        <v>372</v>
       </c>
       <c r="F56" t="s">
-        <v>335</v>
+        <v>295</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3904,16 +3922,16 @@
         <v>103</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>255</v>
+        <v>331</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>297</v>
+        <v>325</v>
       </c>
       <c r="F57" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>14</v>
       </c>
@@ -3924,13 +3942,16 @@
         <v>103</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>363</v>
+        <v>324</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>325</v>
       </c>
       <c r="F58" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>14</v>
       </c>
@@ -3941,10 +3962,16 @@
         <v>103</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+        <v>334</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="F59" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>14</v>
       </c>
@@ -3952,19 +3979,19 @@
         <v>29</v>
       </c>
       <c r="C60" t="s">
-        <v>160</v>
+        <v>103</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>378</v>
+        <v>296</v>
       </c>
       <c r="F60" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>14</v>
       </c>
@@ -3972,19 +3999,16 @@
         <v>29</v>
       </c>
       <c r="C61" t="s">
-        <v>160</v>
+        <v>103</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>379</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>398</v>
+        <v>361</v>
       </c>
       <c r="F61" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>14</v>
       </c>
@@ -3992,19 +4016,13 @@
         <v>29</v>
       </c>
       <c r="C62" t="s">
-        <v>160</v>
+        <v>103</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>380</v>
-      </c>
-      <c r="E62" s="2" t="s">
-        <v>399</v>
-      </c>
-      <c r="F62" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>14</v>
       </c>
@@ -4015,16 +4033,16 @@
         <v>160</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>381</v>
+        <v>256</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>355</v>
+        <v>375</v>
       </c>
       <c r="F63" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>14</v>
       </c>
@@ -4035,16 +4053,16 @@
         <v>160</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>384</v>
+        <v>393</v>
       </c>
       <c r="F64" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" ht="172.8" x14ac:dyDescent="0.3">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>14</v>
       </c>
@@ -4055,13 +4073,13 @@
         <v>160</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>387</v>
+        <v>394</v>
       </c>
       <c r="F65" t="s">
-        <v>187</v>
+        <v>146</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -4075,16 +4093,16 @@
         <v>160</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>386</v>
+        <v>378</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>388</v>
+        <v>353</v>
       </c>
       <c r="F66" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>14</v>
       </c>
@@ -4095,15 +4113,18 @@
         <v>160</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>389</v>
+        <v>379</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>381</v>
       </c>
       <c r="F67" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B68" t="s">
         <v>29</v>
@@ -4112,13 +4133,16 @@
         <v>160</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>390</v>
+        <v>382</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>405</v>
       </c>
       <c r="F68" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>14</v>
       </c>
@@ -4129,13 +4153,16 @@
         <v>160</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>298</v>
+        <v>383</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>384</v>
       </c>
       <c r="F69" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>14</v>
       </c>
@@ -4146,13 +4173,13 @@
         <v>160</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>258</v>
+        <v>385</v>
       </c>
       <c r="F70" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>14</v>
       </c>
@@ -4163,16 +4190,13 @@
         <v>160</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="E71" s="2" t="s">
-        <v>394</v>
+        <v>386</v>
       </c>
       <c r="F71" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>14</v>
       </c>
@@ -4183,16 +4207,13 @@
         <v>160</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>396</v>
-      </c>
-      <c r="E72" t="s">
-        <v>395</v>
+        <v>297</v>
       </c>
       <c r="F72" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>14</v>
       </c>
@@ -4203,16 +4224,13 @@
         <v>160</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>397</v>
-      </c>
-      <c r="E73" t="s">
-        <v>395</v>
+        <v>257</v>
       </c>
       <c r="F73" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>14</v>
       </c>
@@ -4223,16 +4241,16 @@
         <v>160</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>376</v>
+        <v>406</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>377</v>
+        <v>390</v>
       </c>
       <c r="F74" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>14</v>
       </c>
@@ -4243,15 +4261,18 @@
         <v>160</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>259</v>
+        <v>392</v>
+      </c>
+      <c r="E75" t="s">
+        <v>391</v>
       </c>
       <c r="F75" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B76" t="s">
         <v>29</v>
@@ -4260,15 +4281,18 @@
         <v>160</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>364</v>
+        <v>407</v>
+      </c>
+      <c r="E76" t="s">
+        <v>391</v>
       </c>
       <c r="F76" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B77" t="s">
         <v>29</v>
@@ -4277,10 +4301,13 @@
         <v>160</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>400</v>
+        <v>374</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>404</v>
       </c>
       <c r="F77" t="s">
-        <v>401</v>
+        <v>255</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4294,13 +4321,13 @@
         <v>160</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>303</v>
+        <v>258</v>
       </c>
       <c r="F78" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>14</v>
       </c>
@@ -4311,13 +4338,13 @@
         <v>160</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>304</v>
+        <v>362</v>
       </c>
       <c r="F79" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>14</v>
       </c>
@@ -4328,13 +4355,13 @@
         <v>160</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>365</v>
+        <v>395</v>
       </c>
       <c r="F80" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>14</v>
       </c>
@@ -4342,16 +4369,13 @@
         <v>29</v>
       </c>
       <c r="C81" t="s">
-        <v>108</v>
+        <v>160</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>366</v>
-      </c>
-      <c r="E81" s="2" t="s">
-        <v>168</v>
+        <v>301</v>
       </c>
       <c r="F81" t="s">
-        <v>144</v>
+        <v>300</v>
       </c>
     </row>
     <row r="82" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4362,16 +4386,13 @@
         <v>29</v>
       </c>
       <c r="C82" t="s">
-        <v>108</v>
+        <v>160</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="E82" s="2" t="s">
-        <v>265</v>
+        <v>302</v>
       </c>
       <c r="F82" t="s">
-        <v>146</v>
+        <v>299</v>
       </c>
     </row>
     <row r="83" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4382,19 +4403,16 @@
         <v>29</v>
       </c>
       <c r="C83" t="s">
-        <v>108</v>
+        <v>160</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="E83" s="2" t="s">
-        <v>172</v>
+        <v>363</v>
       </c>
       <c r="F83" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>14</v>
       </c>
@@ -4405,16 +4423,16 @@
         <v>108</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>167</v>
+        <v>364</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="F84" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>14</v>
       </c>
@@ -4425,13 +4443,13 @@
         <v>108</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>270</v>
+        <v>163</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="F85" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="86" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4445,16 +4463,16 @@
         <v>108</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>316</v>
+        <v>366</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>195</v>
+        <v>172</v>
       </c>
       <c r="F86" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>14</v>
       </c>
@@ -4465,13 +4483,16 @@
         <v>108</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>194</v>
+        <v>167</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>172</v>
       </c>
       <c r="F87" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>14</v>
       </c>
@@ -4482,13 +4503,13 @@
         <v>108</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>369</v>
+        <v>269</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>276</v>
+        <v>262</v>
       </c>
       <c r="F88" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="89" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4502,16 +4523,16 @@
         <v>108</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>369</v>
+        <v>314</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>277</v>
+        <v>195</v>
       </c>
       <c r="F89" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>14</v>
       </c>
@@ -4522,16 +4543,13 @@
         <v>108</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="E90" s="2" t="s">
-        <v>278</v>
+        <v>194</v>
       </c>
       <c r="F90" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>14</v>
       </c>
@@ -4542,16 +4560,16 @@
         <v>108</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>357</v>
+        <v>367</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>262</v>
+        <v>275</v>
       </c>
       <c r="F91" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>14</v>
       </c>
@@ -4562,16 +4580,16 @@
         <v>108</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>261</v>
+        <v>367</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>262</v>
+        <v>276</v>
       </c>
       <c r="F92" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>14</v>
       </c>
@@ -4582,16 +4600,16 @@
         <v>108</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>268</v>
+        <v>273</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>267</v>
+        <v>277</v>
       </c>
       <c r="F93" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>14</v>
       </c>
@@ -4602,16 +4620,16 @@
         <v>108</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>269</v>
+        <v>355</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
       <c r="F94" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" ht="216" x14ac:dyDescent="0.3">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>14</v>
       </c>
@@ -4622,16 +4640,16 @@
         <v>108</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>193</v>
+        <v>260</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>315</v>
+        <v>261</v>
       </c>
       <c r="F95" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>14</v>
       </c>
@@ -4642,13 +4660,16 @@
         <v>108</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>305</v>
+        <v>267</v>
+      </c>
+      <c r="E96" s="2" t="s">
+        <v>266</v>
       </c>
       <c r="F96" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>14</v>
       </c>
@@ -4659,13 +4680,16 @@
         <v>108</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>312</v>
+        <v>268</v>
+      </c>
+      <c r="E97" s="2" t="s">
+        <v>272</v>
       </c>
       <c r="F97" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" ht="216" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>14</v>
       </c>
@@ -4676,13 +4700,16 @@
         <v>108</v>
       </c>
       <c r="D98" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="E98" s="2" t="s">
         <v>313</v>
       </c>
       <c r="F98" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>14</v>
       </c>
@@ -4693,13 +4720,13 @@
         <v>108</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>279</v>
+        <v>303</v>
       </c>
       <c r="F99" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>14</v>
       </c>
@@ -4707,16 +4734,13 @@
         <v>29</v>
       </c>
       <c r="C100" t="s">
-        <v>213</v>
+        <v>108</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="E100" s="2" t="s">
-        <v>282</v>
+        <v>310</v>
       </c>
       <c r="F100" t="s">
-        <v>144</v>
+        <v>308</v>
       </c>
     </row>
     <row r="101" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4727,19 +4751,16 @@
         <v>29</v>
       </c>
       <c r="C101" t="s">
-        <v>213</v>
+        <v>108</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="E101" s="2" t="s">
-        <v>350</v>
+        <v>311</v>
       </c>
       <c r="F101" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>14</v>
       </c>
@@ -4747,19 +4768,16 @@
         <v>29</v>
       </c>
       <c r="C102" t="s">
-        <v>213</v>
+        <v>108</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="E102" s="2" t="s">
-        <v>350</v>
+        <v>278</v>
       </c>
       <c r="F102" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>14</v>
       </c>
@@ -4767,16 +4785,16 @@
         <v>29</v>
       </c>
       <c r="C103" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>289</v>
+        <v>218</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>351</v>
+        <v>281</v>
       </c>
       <c r="F103" t="s">
-        <v>286</v>
+        <v>144</v>
       </c>
     </row>
     <row r="104" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4787,74 +4805,134 @@
         <v>29</v>
       </c>
       <c r="C104" t="s">
+        <v>212</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="E104" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="F104" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>14</v>
+      </c>
+      <c r="B105" t="s">
+        <v>29</v>
+      </c>
+      <c r="C105" t="s">
+        <v>212</v>
+      </c>
+      <c r="D105" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="E105" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="F105" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>14</v>
+      </c>
+      <c r="B106" t="s">
+        <v>29</v>
+      </c>
+      <c r="C106" t="s">
+        <v>212</v>
+      </c>
+      <c r="D106" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="E106" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="F106" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>14</v>
+      </c>
+      <c r="B107" t="s">
+        <v>29</v>
+      </c>
+      <c r="C107" t="s">
+        <v>212</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="E107" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="F107" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>14</v>
+      </c>
+      <c r="B108" t="s">
+        <v>29</v>
+      </c>
+      <c r="C108" t="s">
+        <v>212</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="E108" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="F108" t="s">
         <v>213</v>
       </c>
-      <c r="D104" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="E104" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="F104" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A105" t="s">
-        <v>14</v>
-      </c>
-      <c r="B105" t="s">
-        <v>29</v>
-      </c>
-      <c r="C105" t="s">
-        <v>213</v>
-      </c>
-      <c r="D105" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="E105" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="F105" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A106" t="s">
-        <v>14</v>
-      </c>
-      <c r="B106" t="s">
-        <v>29</v>
-      </c>
-      <c r="C106" t="s">
-        <v>213</v>
-      </c>
-      <c r="D106" s="2" t="s">
-        <v>338</v>
-      </c>
-      <c r="F106" t="s">
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>14</v>
+      </c>
+      <c r="B109" t="s">
+        <v>29</v>
+      </c>
+      <c r="C109" t="s">
+        <v>212</v>
+      </c>
+      <c r="D109" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="F109" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>14</v>
+      </c>
+      <c r="B110" t="s">
+        <v>29</v>
+      </c>
+      <c r="C110" t="s">
+        <v>212</v>
+      </c>
+      <c r="D110" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="F110" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="107" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A107" t="s">
-        <v>14</v>
-      </c>
-      <c r="B107" t="s">
-        <v>29</v>
-      </c>
-      <c r="C107" t="s">
-        <v>213</v>
-      </c>
-      <c r="D107" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="F107" t="s">
-        <v>284</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:F132">
+  <conditionalFormatting sqref="B3:F135">
     <cfRule type="expression" dxfId="12" priority="1">
       <formula>$A3="No"</formula>
     </cfRule>
@@ -5158,13 +5236,13 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
+        <v>214</v>
+      </c>
+      <c r="C9" t="s">
         <v>215</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>216</v>
-      </c>
-      <c r="D9" t="s">
-        <v>217</v>
       </c>
     </row>
   </sheetData>

</xml_diff>